<commit_message>
Updated test_states.xlsx and tes_states.r
</commit_message>
<xml_diff>
--- a/inst/test_cases/test_states.xlsx
+++ b/inst/test_cases/test_states.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander_lonshteyn/Desktop/HeRomod2/heRomod2/inst/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DDA839-253C-4D4D-B34B-F61300807CCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3600D9-3433-7045-A019-F5E7B3F39BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="500" windowWidth="18740" windowHeight="14280" activeTab="1" xr2:uid="{1CD1D798-17AD-2444-90E8-7015437772F4}"/>
   </bookViews>
   <sheets>
     <sheet name="setting" sheetId="3" r:id="rId1"/>
-    <sheet name="names" sheetId="2" r:id="rId2"/>
-    <sheet name="states" sheetId="1" r:id="rId3"/>
+    <sheet name="wrong_name" sheetId="6" r:id="rId2"/>
+    <sheet name="miss_name" sheetId="5" r:id="rId3"/>
+    <sheet name="dup_names" sheetId="2" r:id="rId4"/>
+    <sheet name="states" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="34">
   <si>
     <t>relapse_free_on_tx</t>
   </si>
@@ -893,11 +895,357 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D695BC0-B4D9-B144-8674-2FA52E62DA0E}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>12</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939B5602-E4BE-0E47-844C-F6125CE3850B}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>12</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F2DC91-071B-B94A-93CA-A84E3E2B0E77}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D742748-4F30-B349-91CD-2BA653A486FE}">
   <dimension ref="A1:H26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update with adding conditions to parse states
</commit_message>
<xml_diff>
--- a/inst/test_cases/test_states.xlsx
+++ b/inst/test_cases/test_states.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander_lonshteyn/Desktop/HeRomod2/heRomod2/inst/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3600D9-3433-7045-A019-F5E7B3F39BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2829C7-7C0C-524E-88B8-597C72450BCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="18740" windowHeight="14280" activeTab="1" xr2:uid="{1CD1D798-17AD-2444-90E8-7015437772F4}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="18740" windowHeight="14280" activeTab="4" xr2:uid="{1CD1D798-17AD-2444-90E8-7015437772F4}"/>
   </bookViews>
   <sheets>
     <sheet name="setting" sheetId="3" r:id="rId1"/>
     <sheet name="wrong_name" sheetId="6" r:id="rId2"/>
     <sheet name="miss_name" sheetId="5" r:id="rId3"/>
     <sheet name="dup_names" sheetId="2" r:id="rId4"/>
-    <sheet name="states" sheetId="1" r:id="rId5"/>
+    <sheet name="reserved" sheetId="8" r:id="rId5"/>
+    <sheet name="probab" sheetId="7" r:id="rId6"/>
+    <sheet name="states" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="35">
   <si>
     <t>relapse_free_on_tx</t>
   </si>
@@ -131,6 +133,9 @@
   </si>
   <si>
     <t>state_cycle_limit_unit</t>
+  </si>
+  <si>
+    <t>cycle</t>
   </si>
 </sst>
 </file>
@@ -898,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D695BC0-B4D9-B144-8674-2FA52E62DA0E}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -907,6 +912,9 @@
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1413,6 +1421,670 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856D7167-0A16-1D46-9DF5-AC592D7D1CED}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>12</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A049CCF2-EE74-A244-8934-4725A4357A6E}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>12</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D742748-4F30-B349-91CD-2BA653A486FE}">
   <dimension ref="A1:H26"/>
   <sheetViews>

</xml_diff>